<commit_message>
Added all approved papers from review meeting 1 & 2.
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>DOI</t>
   </si>
@@ -57,38 +57,359 @@
     <t>E</t>
   </si>
   <si>
-    <t>The title of an interesting paper found on the topic of MVR</t>
-  </si>
-  <si>
-    <t>chemical, recompression</t>
-  </si>
-  <si>
-    <t>http://dontclickthislink.com</t>
-  </si>
-  <si>
-    <t>foo.pdf</t>
-  </si>
-  <si>
     <t>read</t>
   </si>
   <si>
-    <t>This is another paper with a slightly  different take on the topic</t>
-  </si>
-  <si>
-    <t>recompression,</t>
-  </si>
-  <si>
-    <t>bar.pdf</t>
-  </si>
-  <si>
     <t>drop</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>Synergy of electrification and energy efficiency improvement via vapor recompression heat pump and heat exchanger network to achieve decarbonization of extractive distillation</t>
+  </si>
+  <si>
+    <t>Charge source and the charging mechanism of the contact electrification of polymer powder</t>
+  </si>
+  <si>
+    <t>Chemical electrification at solid/liquid/air interface by surface dipole of self-assembled monolayer and harvesting energy of moving water</t>
+  </si>
+  <si>
+    <t>Electrical-driven self-heat recuperative pressure-swing azeotropic distillation to minimize process cost and CO2 emission: Process electrification and simultaneous optimization,</t>
+  </si>
+  <si>
+    <r>
+      <t>Power-to-ammonia in future North European 100 % renewable power and heat system, International Journal of Hydrogen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Energy,Volume 43, Issue 36,2018,Pages 17295-17308, ISSN 0360-3199</t>
+    </r>
+  </si>
+  <si>
+    <t>Electrifying the nitrogen cycle: An electrochemical endeavor, Current Opinion in Electrochemistry, Volume 30, 2021,100790, ISSN 2451-9103,</t>
+  </si>
+  <si>
+    <t>Simultaneous optimization of economic, environmental and safety criteria for algal biodiesel process retrofitted using dividing wall column and multistage vapor recompression,</t>
+  </si>
+  <si>
+    <r>
+      <t>A novel absorption-based enclosed heat pump dryer with combining liquid desiccant dehumidification and mechanical vapor recompressio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">n: Case study and performance evaluation </t>
+    </r>
+  </si>
+  <si>
+    <t>Experimental and numerical study on thermodynamic characteristics of a vacuum membrane distillation system based on mechanical vapor recompression for sulfuric acid waste</t>
+  </si>
+  <si>
+    <t>Energy saving alternatives for renewable ethanol production with the focus on separation/purification units: A techno-economic analysis, Energy, Volume 239, Part E,2022,122363,ISSN 0360-5442,</t>
+  </si>
+  <si>
+    <r>
+      <t>Split Heat Pump Distillation Based on Two-Stage Compression for Separating an Acetone-Water Mixture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ; Chemical Engineering and Technology Volume 45, Issue 1, Pages 159 - 166January 2022</t>
+    </r>
+  </si>
+  <si>
+    <t>A Heat-Integrated Reactive Distillation Process for Methyl Lactate Hydrolysis, Chemical Engineering and Processing - Process Intensification, Volume 170, 2022, 108695, ISSN 0255-2701,</t>
+  </si>
+  <si>
+    <t>Exergy investigation of three ideal regeneration methods for liquid desiccant: Thermal air, mechanical vapor recompression and electrodialysis regeneration, Energy and Buildings,Volume 249,2021, 111258, ISSN 0378-7788,</t>
+  </si>
+  <si>
+    <t>Characteristics analysis of a combined system of vacuum membrane distillation and mechanical vapor recompression; Zetian Si, Dong Han*, Jiming Gu, Yan Song, Pengpeng Zhang</t>
+  </si>
+  <si>
+    <t>Energetic and exergetic analysis of evaporation desalination system integrated with mechanical vapor recompression circulation</t>
+  </si>
+  <si>
+    <t>Evaluation of mechanical vapor recompression crystallization process for treatment of high salinity wastewater,</t>
+  </si>
+  <si>
+    <t>Enhancement of a R-410A Reclamation Process Using Various Heat-Pump-Assisted Distillation Configurations" Energies 12, no. 19: 3776.</t>
+  </si>
+  <si>
+    <t>Novel Process Design Combined with Reactive Distillation and Pressure-Swing Distillation for Propylene Glycol Monomethyl Ether Acetate Synthesis</t>
+  </si>
+  <si>
+    <t>Analysis of heat integration, intermediate reboiler and vapor recompression for the extractive distillation of ternary mixture with two binary azeotropes</t>
+  </si>
+  <si>
+    <r>
+      <t>Microwave-assisted chemical recycling for polymeric waste valorisation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Electrifying Organic Synthesis</t>
+  </si>
+  <si>
+    <t>Current state of industrial heating and opportunities for decarbonization</t>
+  </si>
+  <si>
+    <t>Induction heating as an alternative electrified heating method for carbon capture process</t>
+  </si>
+  <si>
+    <t>Studies on the conceptual design of energy recovery and utility systems for electrified chemical processes</t>
+  </si>
+  <si>
+    <t>Environmental management of industrial decarbonization with focus on chemical sectors: A review</t>
+  </si>
+  <si>
+    <t>Integration of energy systems</t>
+  </si>
+  <si>
+    <t>Saving energy in China’s industry with a focus on electricity: a review of opportunities, potentials and environmental benefits</t>
+  </si>
+  <si>
+    <t>Electrochemical carbon dioxide capture to close the carbon cycle</t>
+  </si>
+  <si>
+    <t>Power-to-methanol: The role of process flexibility in the integration of variable renewable energy into chemical production</t>
+  </si>
+  <si>
+    <t>A general vision for reduction of energy consumption and CO2 emissions from the steel industry</t>
+  </si>
+  <si>
+    <t>Bottom–Up Assessment Framework for Electrification Options in Energy-Intensive Process Industries</t>
+  </si>
+  <si>
+    <t>Electrification of the chemical industry</t>
+  </si>
+  <si>
+    <t>Technologies and policies to decarbonize global industry: Review and assessment of mitigation drivers through 2070</t>
+  </si>
+  <si>
+    <t>Electrical-driven self-heat recuperative pressure-swing azeotropic distillation to minimize process cost and CO2 emission: Process electrification and simultaneous optimization</t>
+  </si>
+  <si>
+    <t>Direct and indirect electrification of chemical industry using methanol production as a case study</t>
+  </si>
+  <si>
+    <t>Recent advances in industrial CO 2 electroreduction</t>
+  </si>
+  <si>
+    <t>Emerging opportunities for electrochemical processing to enable sustainable chemical manufacturing</t>
+  </si>
+  <si>
+    <t>Factoring environment into electrification management in a region</t>
+  </si>
+  <si>
+    <t>Electrification of alkylation process with high speed motor drive system in a refinery</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.seppur.2022.121065</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.apt.2022.103628</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jcis.2022.01.114</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.energy.2020.116998.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijhydene.2018.06.121.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.coelec.2021.100790.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.psep.2022.05.059.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.csite.2022.102091.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cep.2022.108862.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.energy.2021.122363.</t>
+  </si>
+  <si>
+    <t>DOI: 10.1002/ceat.202100289</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cep.2021.108695</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.enbuild.2021.111258.</t>
+  </si>
+  <si>
+    <t>doi: 10.5004/dwt.2019.24781</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.csite.2019.100548</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cep.2019.107682</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/en12193776</t>
+  </si>
+  <si>
+    <t>DOI: 10.1021/acs.iecr.9b04122</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cep.2019.107546.</t>
+  </si>
+  <si>
+    <t>doi: 10.23919/EuMC50147.2022.9784259.</t>
+  </si>
+  <si>
+    <t>DOI: 10.1002/anie.201711060</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.pecs.2021.100982</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cej.2021.133380.</t>
+  </si>
+  <si>
+    <t>10.1016/j.rser.2022.112718</t>
+  </si>
+  <si>
+    <t>10.1016/j.jenvman.2021.114055</t>
+  </si>
+  <si>
+    <t>10.1557/s43577-021-00244-8</t>
+  </si>
+  <si>
+    <t>10.1007/s12053-021-09979-4</t>
+  </si>
+  <si>
+    <t>10.1039/d0ee03382k</t>
+  </si>
+  <si>
+    <t>10.1016/j.enconman.2020.113673</t>
+  </si>
+  <si>
+    <t>10.3390/met10091117</t>
+  </si>
+  <si>
+    <t>10.3389/fenrg.2020.00192</t>
+  </si>
+  <si>
+    <t>10.1126/science.abb8061</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.apenergy.2020.114848</t>
+  </si>
+  <si>
+    <t>10.1016/j.energy.2020.116998</t>
+  </si>
+  <si>
+    <t>10.1016/j.apenergy.2019.03.184</t>
+  </si>
+  <si>
+    <t>10.1016/j.cogsc.2019.01.005</t>
+  </si>
+  <si>
+    <t>10.1016/j.coche.2018.05.002</t>
+  </si>
+  <si>
+    <t>10.2495/SDP-V13-N4-707-717</t>
+  </si>
+  <si>
+    <t>10.1109/PCICON.2015.7435129</t>
+  </si>
+  <si>
+    <t>10.1016/j.seppur.2022.121065</t>
+  </si>
+  <si>
+    <t>PN_8.pdf</t>
+  </si>
+  <si>
+    <t>PN_11.pdf</t>
+  </si>
+  <si>
+    <t>PN_14.pdf</t>
+  </si>
+  <si>
+    <t>PN_15.pdf</t>
+  </si>
+  <si>
+    <t>PN_17.pdf</t>
+  </si>
+  <si>
+    <t>PN_18.pdf</t>
+  </si>
+  <si>
+    <t>PN_21.pdf</t>
+  </si>
+  <si>
+    <t>PN_22.pdf</t>
+  </si>
+  <si>
+    <t>PN_23.pdf</t>
+  </si>
+  <si>
+    <t>PN_26.pdf</t>
+  </si>
+  <si>
+    <t>PN_27.pdf</t>
+  </si>
+  <si>
+    <t>PN_28.pdf</t>
+  </si>
+  <si>
+    <t>PN_30.pdf</t>
+  </si>
+  <si>
+    <t>PN_31.pdf</t>
+  </si>
+  <si>
+    <t>PN_32.pdf</t>
+  </si>
+  <si>
+    <t>PN_33.pdf</t>
+  </si>
+  <si>
+    <t>PN_37.pdf</t>
+  </si>
+  <si>
+    <t>PN_38.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +425,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF2E74B5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,15 +483,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -148,16 +550,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L1048576" totalsRowShown="0">
-  <autoFilter ref="A1:L1048576"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M1048576" totalsRowShown="0">
+  <autoFilter ref="A1:M1048576"/>
+  <tableColumns count="13">
+    <tableColumn id="13" name="PN"/>
     <tableColumn id="1" name="TITLE"/>
-    <tableColumn id="2" name="TAGS"/>
-    <tableColumn id="3" name="DOI"/>
-    <tableColumn id="4" name="LINK"/>
-    <tableColumn id="5" name="SOURCES"/>
-    <tableColumn id="6" name="NOTES"/>
-    <tableColumn id="7" name="STATUS"/>
+    <tableColumn id="2" name="TAGS" dataDxfId="5"/>
+    <tableColumn id="3" name="DOI" dataDxfId="4"/>
+    <tableColumn id="4" name="LINK" dataDxfId="3"/>
+    <tableColumn id="5" name="SOURCES" dataDxfId="2"/>
+    <tableColumn id="6" name="NOTES" dataDxfId="1"/>
+    <tableColumn id="7" name="STATUS" dataDxfId="0"/>
     <tableColumn id="8" name="A"/>
     <tableColumn id="9" name="B"/>
     <tableColumn id="10" name="C"/>
@@ -431,101 +834,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
+    <col min="8" max="8" width="13.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="B27" r:id="rId1" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85122285462&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=6&amp;citeCnt=1&amp;searchTerm="/>
+    <hyperlink ref="B28" r:id="rId2" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85111382489&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=9&amp;citeCnt=3&amp;searchTerm="/>
+    <hyperlink ref="B29" r:id="rId3" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85101222848&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=10&amp;citeCnt=47&amp;searchTerm="/>
+    <hyperlink ref="B30" r:id="rId4" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85097438807&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=11&amp;citeCnt=21&amp;searchTerm="/>
+    <hyperlink ref="B31" r:id="rId5" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85089702026&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=13&amp;citeCnt=32&amp;searchTerm="/>
+    <hyperlink ref="B32" r:id="rId6" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85090024597&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=16&amp;citeCnt=4&amp;searchTerm="/>
+    <hyperlink ref="B33" r:id="rId7" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85086424435&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=17&amp;citeCnt=20&amp;searchTerm="/>
+    <hyperlink ref="E2" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="E4" r:id="rId10" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="E18" r:id="rId11"/>
+    <hyperlink ref="E25" r:id="rId12" display="https://doi.org/10.1016/j.rser.2022.112718"/>
+    <hyperlink ref="E26" r:id="rId13" display="https://doi.org/10.1016/j.jenvman.2021.114055"/>
+    <hyperlink ref="E27" r:id="rId14" display="https://doi.org/10.1557/s43577-021-00244-8"/>
+    <hyperlink ref="E28" r:id="rId15" display="https://doi.org/10.1007/s12053-021-09979-4"/>
+    <hyperlink ref="E29" r:id="rId16" display="https://doi.org/10.1039/d0ee03382k"/>
+    <hyperlink ref="E30" r:id="rId17" display="https://doi.org/10.1016/j.enconman.2020.113673"/>
+    <hyperlink ref="E31" r:id="rId18" display="https://doi.org/10.3390/met10091117"/>
+    <hyperlink ref="E32" r:id="rId19" display="https://doi.org/10.3389/fenrg.2020.00192"/>
+    <hyperlink ref="E33" r:id="rId20" display="https://doi.org/10.1126/science.abb8061"/>
+    <hyperlink ref="E34" r:id="rId21" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="E37" r:id="rId22" display="https://doi.org/10.1016/j.cogsc.2019.01.005"/>
+    <hyperlink ref="E38" r:id="rId23" display="https://doi.org/10.1016/j.coche.2018.05.002"/>
+    <hyperlink ref="E39" r:id="rId24" display="https://doi.org/10.2495/SDP-V13-N4-707-717"/>
+    <hyperlink ref="E40" r:id="rId25" display="https://doi.org/10.1109/PCICON.2015.7435129"/>
+    <hyperlink ref="E24" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded remaining papers - not from TU access. Updated DOI's.
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
   <si>
     <t>DOI</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>read</t>
-  </si>
-  <si>
-    <t>drop</t>
   </si>
   <si>
     <t>PN</t>
@@ -213,9 +207,6 @@
     <t>Technologies and policies to decarbonize global industry: Review and assessment of mitigation drivers through 2070</t>
   </si>
   <si>
-    <t>Electrical-driven self-heat recuperative pressure-swing azeotropic distillation to minimize process cost and CO2 emission: Process electrification and simultaneous optimization</t>
-  </si>
-  <si>
     <t>Direct and indirect electrification of chemical industry using methanol production as a case study</t>
   </si>
   <si>
@@ -403,13 +394,139 @@
   </si>
   <si>
     <t>PN_38.pdf</t>
+  </si>
+  <si>
+    <t>PN_1.pdf</t>
+  </si>
+  <si>
+    <t>PN_2.pdf</t>
+  </si>
+  <si>
+    <t>PN_3.pdf</t>
+  </si>
+  <si>
+    <t>PN_4.pdf</t>
+  </si>
+  <si>
+    <t>PN_5.pdf</t>
+  </si>
+  <si>
+    <t>PN_6.pdf</t>
+  </si>
+  <si>
+    <t>PN_7.pdf</t>
+  </si>
+  <si>
+    <t>PN_9.pdf</t>
+  </si>
+  <si>
+    <t>PN_10.pdf</t>
+  </si>
+  <si>
+    <t>PN_12.pdf</t>
+  </si>
+  <si>
+    <t>PN_13.pdf</t>
+  </si>
+  <si>
+    <t>PN_16.pdf</t>
+  </si>
+  <si>
+    <t>PN_19.pdf</t>
+  </si>
+  <si>
+    <t>PN_20.pdf</t>
+  </si>
+  <si>
+    <t>PN_24.pdf</t>
+  </si>
+  <si>
+    <t>PN_25.pdf</t>
+  </si>
+  <si>
+    <t>PN_29.pdf</t>
+  </si>
+  <si>
+    <t>PN_35.pdf</t>
+  </si>
+  <si>
+    <t>PN_36.pdf</t>
+  </si>
+  <si>
+    <t>PN_39.pdf</t>
+  </si>
+  <si>
+    <t>10.1016/j.apt.2022.103628</t>
+  </si>
+  <si>
+    <t>10.1016/j.jcis.2022.01.114</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijhydene.2018.06.121</t>
+  </si>
+  <si>
+    <t>10.1016/j.coelec.2021.100790</t>
+  </si>
+  <si>
+    <t>10.1016/j.psep.2022.05.059</t>
+  </si>
+  <si>
+    <t>10.1016/j.csite.2022.102091</t>
+  </si>
+  <si>
+    <t>10.1016/j.cep.2022.108862</t>
+  </si>
+  <si>
+    <t>10.1016/j.energy.2021.122363</t>
+  </si>
+  <si>
+    <t>10.1002/ceat.202100289</t>
+  </si>
+  <si>
+    <t>10.1016/j.cep.2021.108695</t>
+  </si>
+  <si>
+    <t>10.1016/j.enbuild.2021.111258</t>
+  </si>
+  <si>
+    <t>10.5004/dwt.2019.24781</t>
+  </si>
+  <si>
+    <t>10.1016/j.csite.2019.100548</t>
+  </si>
+  <si>
+    <t>10.3390/en12193776</t>
+  </si>
+  <si>
+    <t>10.1016/j.cep.2019.107682</t>
+  </si>
+  <si>
+    <t>10.1021/acs.iecr.9b04122</t>
+  </si>
+  <si>
+    <t>10.1016/j.cep.2019.107546</t>
+  </si>
+  <si>
+    <t>10.23919/EuMC50147.2022.9784259</t>
+  </si>
+  <si>
+    <t>10.1002/anie.201711060</t>
+  </si>
+  <si>
+    <t>10.1016/j.pecs.2021.100982</t>
+  </si>
+  <si>
+    <t>10.1016/j.cej.2021.133380</t>
+  </si>
+  <si>
+    <t>10.1016/j.apenergy.2020.114848</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,14 +543,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,9 +551,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF2E74B5"/>
+      <color rgb="FF404040"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -483,14 +591,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -500,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -509,7 +611,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M1048576" totalsRowShown="0">
-  <autoFilter ref="A1:M1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M1048575" totalsRowShown="0">
+  <autoFilter ref="A1:M1048575"/>
   <tableColumns count="13">
     <tableColumn id="13" name="PN"/>
     <tableColumn id="1" name="TITLE"/>
@@ -834,47 +939,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="70.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="7"/>
-    <col min="8" max="8" width="13.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="13.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
@@ -894,495 +999,649 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="B30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="B32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>35</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="B35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>36</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="B36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>37</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>38</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="B38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>39</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="D39" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>38</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>92</v>
+      <c r="E39" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1654,8 @@
     <hyperlink ref="B32" r:id="rId6" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85090024597&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=16&amp;citeCnt=4&amp;searchTerm="/>
     <hyperlink ref="B33" r:id="rId7" tooltip="Show document details" display="https://www.scopus.com/record/display.uri?eid=2-s2.0-85086424435&amp;origin=resultslist&amp;sort=plfdt-f&amp;listId=57701981&amp;listTypeValue=Docs&amp;src=s&amp;imp=t&amp;sid=246a5f5a1833d2f2bce75e1ee34c5b6a&amp;sot=sl&amp;sdt=sl&amp;sl=0&amp;relpos=17&amp;citeCnt=20&amp;searchTerm="/>
     <hyperlink ref="E2" r:id="rId8"/>
-    <hyperlink ref="E3" r:id="rId9" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="E4" r:id="rId10" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E4" r:id="rId10"/>
     <hyperlink ref="E18" r:id="rId11"/>
     <hyperlink ref="E25" r:id="rId12" display="https://doi.org/10.1016/j.rser.2022.112718"/>
     <hyperlink ref="E26" r:id="rId13" display="https://doi.org/10.1016/j.jenvman.2021.114055"/>
@@ -1408,15 +1667,27 @@
     <hyperlink ref="E32" r:id="rId19" display="https://doi.org/10.3389/fenrg.2020.00192"/>
     <hyperlink ref="E33" r:id="rId20" display="https://doi.org/10.1126/science.abb8061"/>
     <hyperlink ref="E34" r:id="rId21" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="E37" r:id="rId22" display="https://doi.org/10.1016/j.cogsc.2019.01.005"/>
-    <hyperlink ref="E38" r:id="rId23" display="https://doi.org/10.1016/j.coche.2018.05.002"/>
-    <hyperlink ref="E39" r:id="rId24" display="https://doi.org/10.2495/SDP-V13-N4-707-717"/>
-    <hyperlink ref="E40" r:id="rId25" display="https://doi.org/10.1109/PCICON.2015.7435129"/>
+    <hyperlink ref="E36" r:id="rId22" display="https://doi.org/10.1016/j.cogsc.2019.01.005"/>
+    <hyperlink ref="E37" r:id="rId23" display="https://doi.org/10.1016/j.coche.2018.05.002"/>
+    <hyperlink ref="E38" r:id="rId24" display="https://doi.org/10.2495/SDP-V13-N4-707-717"/>
+    <hyperlink ref="E39" r:id="rId25" display="https://doi.org/10.1109/PCICON.2015.7435129"/>
     <hyperlink ref="E24" r:id="rId26"/>
+    <hyperlink ref="E5" r:id="rId27"/>
+    <hyperlink ref="E6" r:id="rId28"/>
+    <hyperlink ref="E7" r:id="rId29"/>
+    <hyperlink ref="E8" r:id="rId30"/>
+    <hyperlink ref="E9" r:id="rId31"/>
+    <hyperlink ref="E10" r:id="rId32"/>
+    <hyperlink ref="E11" r:id="rId33"/>
+    <hyperlink ref="E13" r:id="rId34"/>
+    <hyperlink ref="E14" r:id="rId35"/>
+    <hyperlink ref="E16" r:id="rId36"/>
+    <hyperlink ref="E17" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId39"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>